<commit_message>
fixed typo in homelessness_analysis
</commit_message>
<xml_diff>
--- a/BoSClean/homelessness.xlsx
+++ b/BoSClean/homelessness.xlsx
@@ -2224,7 +2224,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2235,7 +2235,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Times Homeless in 3 years</t>
+          <t>Months Homeless in 3 years</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -2252,11 +2252,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>One time (HUD)</t>
+          <t>More than 12</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -2267,11 +2267,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Two times (HUD)</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -2282,11 +2282,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Four or more times (HUD)</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2297,11 +2297,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Three times (HUD)</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -2312,11 +2312,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Not Specified</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -2327,120 +2327,120 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>One time (HUD)</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MC</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Four or more times (HUD)</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MC</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Two times (HUD)</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MC</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Three times (HUD)</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MC</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Not Specified</t>
+          <t>7</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>One time (HUD)</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Four or more times (HUD)</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Two times (HUD)</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>SPC</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
@@ -2451,153 +2451,153 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>719</v>
+        <v>1</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>8319</t>
+          <t>OC</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>One time (HUD)</t>
+          <t>More than 12</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>8319</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Four or more times (HUD)</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8319</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Two times (HUD)</t>
+          <t>7</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>8319</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Three times (HUD)</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>8319</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Data not collected (HUD)</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>8319</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>One time (HUD)</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Erin</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Two times (HUD)</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Erin</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Not Specified</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Erin</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Three times (HUD)</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Erin</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Data not collected (HUD)</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -2605,14 +2605,14 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Erin</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Four or more times (HUD)</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -2620,142 +2620,142 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Erin</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Not Specified</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>372</v>
+        <v>1</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>MC</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>One time (HUD)</t>
+          <t>Not Specified</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>268</v>
+        <v>27</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>SPC</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Four or more times (HUD)</t>
+          <t>More than 12</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>110</v>
+        <v>24</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>SPC</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Two times (HUD)</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>83</v>
+        <v>2</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>SPC</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Three times (HUD)</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>SPC</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Data not collected (HUD)</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>SPC</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>One time (HUD)</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>11495</t>
+          <t>SPC</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Two times (HUD)</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>11495</t>
+          <t>SPC</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Four or more times (HUD)</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>11495</t>
+          <t>SPC</t>
         </is>
       </c>
     </row>
@@ -2766,99 +2766,894 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>10</v>
+        <v>718</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>11495</t>
+          <t>8319</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Three times (HUD)</t>
+          <t>More than 12</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>11495</t>
+          <t>8319</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Not Specified</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>163</v>
+        <v>22</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1371</t>
+          <t>8319</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>One time (HUD)</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1371</t>
+          <t>8319</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Four or more times (HUD)</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1371</t>
+          <t>8319</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Two times (HUD)</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1371</t>
+          <t>8319</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Three times (HUD)</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B42" t="n">
+        <v>9</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>8319</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>8</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>8319</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>8</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>8319</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
         <v>7</v>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>8319</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>5</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>8319</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Data not collected (HUD)</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>5</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>8319</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>5</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>8319</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>2</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>8319</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>2</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>8319</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>20</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Erin</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Not Specified</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>14</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Erin</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>6</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Erin</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>4</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Erin</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>4</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Erin</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>More than 12</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>3</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Erin</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>2</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Erin</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>2</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Erin</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Data not collected (HUD)</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Erin</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Erin</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Not Specified</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>373</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>More than 12</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>172</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>56</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>51</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>39</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>36</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>34</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>30</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>23</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>16</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>15</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>10</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>9</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>7</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Not Specified</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>10</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>11495</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>9</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>11495</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>More than 12</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>9</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>11495</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>8</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>11495</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>8</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>11495</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>6</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>11495</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>4</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>11495</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>4</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>11495</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Not Specified</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>163</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>1371</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>More than 12</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>68</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>1371</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>12</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>1371</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>12</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>1371</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>10</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>1371</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>8</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>1371</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>6</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>1371</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>6</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>1371</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>5</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>1371</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>4</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>1371</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>3</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>1371</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>1</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>1371</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>1</v>
+      </c>
+      <c r="C95" t="inlineStr">
         <is>
           <t>1371</t>
         </is>

</xml_diff>